<commit_message>
ADD: sql query for days, dates and names
</commit_message>
<xml_diff>
--- a/participantWorkbook.xlsx
+++ b/participantWorkbook.xlsx
@@ -26,70 +26,70 @@
     <t>Salı</t>
   </si>
   <si>
+    <t>4 Emrullah</t>
+  </si>
+  <si>
+    <t>24/10/2023</t>
+  </si>
+  <si>
+    <t>Çarşamba</t>
+  </si>
+  <si>
+    <t>18 Kübra</t>
+  </si>
+  <si>
+    <t>25/10/2023</t>
+  </si>
+  <si>
+    <t>Perşembe</t>
+  </si>
+  <si>
+    <t>3 Eda</t>
+  </si>
+  <si>
+    <t>26/10/2023</t>
+  </si>
+  <si>
+    <t>Cuma</t>
+  </si>
+  <si>
+    <t>6 Cahit</t>
+  </si>
+  <si>
+    <t>27/10/2023</t>
+  </si>
+  <si>
+    <t>Cumartesi</t>
+  </si>
+  <si>
     <t>8 Ertugrul</t>
   </si>
   <si>
-    <t>24/10/2023</t>
-  </si>
-  <si>
-    <t>Çarşamba</t>
-  </si>
-  <si>
-    <t>4 Emrullah</t>
-  </si>
-  <si>
-    <t>25/10/2023</t>
-  </si>
-  <si>
-    <t>Perşembe</t>
-  </si>
-  <si>
-    <t>6 Cahit</t>
-  </si>
-  <si>
-    <t>26/10/2023</t>
-  </si>
-  <si>
-    <t>Cuma</t>
+    <t>28/10/2023</t>
+  </si>
+  <si>
+    <t>Pazartesi</t>
+  </si>
+  <si>
+    <t>10 Ümmü</t>
+  </si>
+  <si>
+    <t>30/10/2023</t>
   </si>
   <si>
     <t>7 Nurullah</t>
   </si>
   <si>
-    <t>27/10/2023</t>
-  </si>
-  <si>
-    <t>Cumartesi</t>
+    <t>31/10/2023</t>
+  </si>
+  <si>
+    <t>29 Ahmet</t>
+  </si>
+  <si>
+    <t>01/11/2023</t>
   </si>
   <si>
     <t>17 Sinan</t>
-  </si>
-  <si>
-    <t>28/10/2023</t>
-  </si>
-  <si>
-    <t>Pazartesi</t>
-  </si>
-  <si>
-    <t>3 Eda</t>
-  </si>
-  <si>
-    <t>30/10/2023</t>
-  </si>
-  <si>
-    <t>18 Kübra</t>
-  </si>
-  <si>
-    <t>31/10/2023</t>
-  </si>
-  <si>
-    <t>29 Ahmet</t>
-  </si>
-  <si>
-    <t>01/11/2023</t>
-  </si>
-  <si>
-    <t>10 Ümmü</t>
   </si>
   <si>
     <t>02/11/2023</t>

</xml_diff>